<commit_message>
change xml implemenation data type on production values
update implementation data type to 'double' for Capacity_MW,
GrossProduction_MWhr, NetProduction_MWhr, AveragePrice_c_kW-h; was
string for a decimal data type.  This won't appear until next version
release.
</commit_message>
<xml_diff>
--- a/PowerPlantProduction.xlsx
+++ b/PowerPlantProduction.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="345" yWindow="180" windowWidth="15600" windowHeight="6705"/>
+    <workbookView xWindow="204" yWindow="180" windowWidth="17268" windowHeight="7752"/>
   </bookViews>
   <sheets>
     <sheet name="About" sheetId="3" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="321" uniqueCount="200">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="324" uniqueCount="202">
   <si>
     <t>Title</t>
   </si>
@@ -328,9 +328,6 @@
   </si>
   <si>
     <t>URI that identifies a metadata record providing more complete information on provenance of this production report.</t>
-  </si>
-  <si>
-    <t>The year in which the first power plant at the site began operation. Included as search parameter.</t>
   </si>
   <si>
     <t>Easting coordinates, UTM 84. UTM included for convienence.</t>
@@ -665,6 +662,15 @@
   </si>
   <si>
     <t>Copyright © Arizona Geological Survey, 2012</t>
+  </si>
+  <si>
+    <t>The year in which the first power plant at the site began operation. Included as search parameter. Integer to help enforce 'YYYY' value.</t>
+  </si>
+  <si>
+    <t>update implementation data type to 'double' for Capacity_MW, GrossProduction_MWhr, NetProduction_MWhr, AveragePrice_c_kW-h; was string for a decimal data type.  This won't appear until next version release.</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> this is the version that is on schemas.usgin.org as version 0.8</t>
   </si>
 </sst>
 </file>
@@ -2287,7 +2293,7 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="157">
+  <cellXfs count="158">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
@@ -2719,6 +2725,9 @@
     <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
       <protection locked="0"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="5" xfId="30" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
@@ -3140,13 +3149,13 @@
     <xdr:from>
       <xdr:col>2</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>23</xdr:row>
+      <xdr:row>24</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>2</xdr:col>
       <xdr:colOff>819150</xdr:colOff>
-      <xdr:row>24</xdr:row>
+      <xdr:row>25</xdr:row>
       <xdr:rowOff>133350</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -3559,20 +3568,20 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="C2:F33"/>
+  <dimension ref="C2:F34"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B4" workbookViewId="0">
-      <selection activeCell="J14" sqref="J14"/>
+    <sheetView tabSelected="1" topLeftCell="B8" workbookViewId="0">
+      <selection activeCell="E17" sqref="E17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="2" width="9.140625" style="72"/>
-    <col min="3" max="3" width="12.42578125" style="71" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="66.140625" style="72" customWidth="1"/>
-    <col min="5" max="5" width="22.5703125" style="72" customWidth="1"/>
-    <col min="6" max="6" width="11.85546875" style="72" customWidth="1"/>
-    <col min="7" max="16384" width="9.140625" style="72"/>
+    <col min="1" max="2" width="9.109375" style="72"/>
+    <col min="3" max="3" width="12.44140625" style="71" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="66.109375" style="72" customWidth="1"/>
+    <col min="5" max="5" width="22.5546875" style="72" customWidth="1"/>
+    <col min="6" max="6" width="11.88671875" style="72" customWidth="1"/>
+    <col min="7" max="16384" width="9.109375" style="72"/>
   </cols>
   <sheetData>
     <row r="2" spans="3:6" ht="105.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -3581,15 +3590,15 @@
         <v>0</v>
       </c>
       <c r="D3" s="69" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="4" spans="3:6" x14ac:dyDescent="0.25">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="4" spans="3:6" ht="15" x14ac:dyDescent="0.25">
       <c r="C4" s="70" t="s">
         <v>1</v>
       </c>
       <c r="D4" s="68" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="5" spans="3:6" ht="75" x14ac:dyDescent="0.25">
@@ -3597,7 +3606,7 @@
         <v>2</v>
       </c>
       <c r="D5" s="53" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
     </row>
     <row r="6" spans="3:6" ht="45" x14ac:dyDescent="0.25">
@@ -3608,10 +3617,10 @@
         <v>67</v>
       </c>
     </row>
-    <row r="7" spans="3:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="3:6" ht="15" x14ac:dyDescent="0.25">
       <c r="D7" s="66"/>
     </row>
-    <row r="9" spans="3:6" x14ac:dyDescent="0.25">
+    <row r="9" spans="3:6" ht="15" x14ac:dyDescent="0.25">
       <c r="C9" s="65" t="s">
         <v>4</v>
       </c>
@@ -3639,12 +3648,12 @@
         <v>41</v>
       </c>
     </row>
-    <row r="11" spans="3:6" ht="75" x14ac:dyDescent="0.25">
+    <row r="11" spans="3:6" ht="57.6" x14ac:dyDescent="0.3">
       <c r="C11" s="63" t="s">
         <v>66</v>
       </c>
       <c r="D11" s="74" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="E11" s="70" t="s">
         <v>95</v>
@@ -3653,12 +3662,12 @@
         <v>41087</v>
       </c>
     </row>
-    <row r="12" spans="3:6" x14ac:dyDescent="0.25">
+    <row r="12" spans="3:6" x14ac:dyDescent="0.3">
       <c r="C12" s="63" t="s">
+        <v>103</v>
+      </c>
+      <c r="D12" s="74" t="s">
         <v>104</v>
-      </c>
-      <c r="D12" s="74" t="s">
-        <v>105</v>
       </c>
       <c r="E12" s="75" t="s">
         <v>95</v>
@@ -3667,128 +3676,142 @@
         <v>41180</v>
       </c>
     </row>
-    <row r="13" spans="3:6" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="3:6" x14ac:dyDescent="0.3">
       <c r="C13" s="63"/>
       <c r="D13" s="74" t="s">
-        <v>197</v>
-      </c>
-      <c r="E13" s="75" t="s">
-        <v>195</v>
-      </c>
-      <c r="F13" s="60">
+        <v>201</v>
+      </c>
+      <c r="E13" s="75"/>
+      <c r="F13" s="60"/>
+    </row>
+    <row r="14" spans="3:6" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C14" s="63"/>
+      <c r="D14" s="74" t="s">
+        <v>196</v>
+      </c>
+      <c r="E14" s="75" t="s">
+        <v>194</v>
+      </c>
+      <c r="F14" s="60">
         <v>41299</v>
       </c>
     </row>
-    <row r="14" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="C14" s="63"/>
-      <c r="D14" s="75"/>
-      <c r="E14" s="75"/>
-      <c r="F14" s="60"/>
-    </row>
-    <row r="15" spans="3:6" x14ac:dyDescent="0.25">
+    <row r="15" spans="3:6" ht="43.2" x14ac:dyDescent="0.3">
       <c r="C15" s="63"/>
-      <c r="D15" s="75"/>
-      <c r="E15" s="75"/>
-      <c r="F15" s="60"/>
-    </row>
-    <row r="16" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="D15" s="74" t="s">
+        <v>200</v>
+      </c>
+      <c r="E15" s="73" t="s">
+        <v>95</v>
+      </c>
+      <c r="F15" s="145">
+        <v>41403</v>
+      </c>
+    </row>
+    <row r="16" spans="3:6" x14ac:dyDescent="0.3">
       <c r="C16" s="63"/>
       <c r="D16" s="75"/>
       <c r="E16" s="75"/>
       <c r="F16" s="60"/>
     </row>
-    <row r="17" spans="3:6" x14ac:dyDescent="0.25">
+    <row r="17" spans="3:6" x14ac:dyDescent="0.3">
       <c r="C17" s="63"/>
       <c r="D17" s="75"/>
       <c r="E17" s="75"/>
       <c r="F17" s="60"/>
     </row>
-    <row r="18" spans="3:6" x14ac:dyDescent="0.25">
+    <row r="18" spans="3:6" x14ac:dyDescent="0.3">
       <c r="C18" s="63"/>
       <c r="D18" s="75"/>
       <c r="E18" s="75"/>
       <c r="F18" s="60"/>
     </row>
-    <row r="19" spans="3:6" x14ac:dyDescent="0.25">
+    <row r="19" spans="3:6" x14ac:dyDescent="0.3">
       <c r="C19" s="63"/>
       <c r="D19" s="75"/>
       <c r="E19" s="75"/>
       <c r="F19" s="60"/>
     </row>
-    <row r="20" spans="3:6" x14ac:dyDescent="0.25">
+    <row r="20" spans="3:6" x14ac:dyDescent="0.3">
       <c r="C20" s="63"/>
       <c r="D20" s="75"/>
       <c r="E20" s="75"/>
       <c r="F20" s="60"/>
     </row>
-    <row r="21" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="C21" s="70"/>
+    <row r="21" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C21" s="63"/>
       <c r="D21" s="75"/>
       <c r="E21" s="75"/>
       <c r="F21" s="60"/>
     </row>
-    <row r="22" spans="3:6" x14ac:dyDescent="0.25">
+    <row r="22" spans="3:6" x14ac:dyDescent="0.3">
       <c r="C22" s="70"/>
       <c r="D22" s="75"/>
       <c r="E22" s="75"/>
       <c r="F22" s="60"/>
     </row>
-    <row r="24" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="D24" s="118" t="s">
+    <row r="23" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C23" s="70"/>
+      <c r="D23" s="75"/>
+      <c r="E23" s="75"/>
+      <c r="F23" s="60"/>
+    </row>
+    <row r="25" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="D25" s="118" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="26" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="D26" s="119" t="s">
         <v>198</v>
       </c>
     </row>
-    <row r="25" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="D25" s="119" t="s">
-        <v>199</v>
-      </c>
-    </row>
-    <row r="28" spans="3:6" ht="18" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C28" s="72"/>
-      <c r="D28" s="59" t="s">
-        <v>156</v>
-      </c>
-      <c r="E28" s="58"/>
-    </row>
-    <row r="29" spans="3:6" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="C29" s="57"/>
-      <c r="D29" s="56" t="s">
+    <row r="29" spans="3:6" ht="18" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C29" s="72"/>
+      <c r="D29" s="59" t="s">
+        <v>155</v>
+      </c>
+      <c r="E29" s="58"/>
+    </row>
+    <row r="30" spans="3:6" ht="15" thickTop="1" x14ac:dyDescent="0.3">
+      <c r="C30" s="57"/>
+      <c r="D30" s="56" t="s">
         <v>5</v>
       </c>
-      <c r="E29" s="55" t="s">
+      <c r="E30" s="55" t="s">
         <v>6</v>
       </c>
-      <c r="F29" s="54" t="s">
+      <c r="F30" s="54" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="30" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="C30" s="72"/>
-      <c r="D30" s="73"/>
-      <c r="E30" s="74"/>
-      <c r="F30" s="73"/>
-    </row>
-    <row r="31" spans="3:6" x14ac:dyDescent="0.25">
+    <row r="31" spans="3:6" x14ac:dyDescent="0.3">
       <c r="C31" s="72"/>
       <c r="D31" s="73"/>
       <c r="E31" s="74"/>
       <c r="F31" s="73"/>
     </row>
-    <row r="32" spans="3:6" x14ac:dyDescent="0.25">
+    <row r="32" spans="3:6" x14ac:dyDescent="0.3">
       <c r="C32" s="72"/>
       <c r="D32" s="73"/>
       <c r="E32" s="74"/>
       <c r="F32" s="73"/>
     </row>
-    <row r="33" spans="3:6" x14ac:dyDescent="0.25">
+    <row r="33" spans="3:6" x14ac:dyDescent="0.3">
       <c r="C33" s="72"/>
       <c r="D33" s="73"/>
       <c r="E33" s="74"/>
       <c r="F33" s="73"/>
     </row>
+    <row r="34" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C34" s="72"/>
+      <c r="D34" s="73"/>
+      <c r="E34" s="74"/>
+      <c r="F34" s="73"/>
+    </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="D24" r:id="rId1" display="http://creativecommons.org/licenses/by/3.0/"/>
+    <hyperlink ref="D25" r:id="rId1" display="http://creativecommons.org/licenses/by/3.0/"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId2"/>
@@ -3805,167 +3828,167 @@
       <selection activeCell="B20" sqref="B20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="29.140625" style="1" customWidth="1"/>
-    <col min="2" max="2" width="63.140625" style="3" customWidth="1"/>
-    <col min="3" max="3" width="37.7109375" style="1" customWidth="1"/>
-    <col min="4" max="16384" width="8.85546875" style="1"/>
+    <col min="1" max="1" width="29.109375" style="1" customWidth="1"/>
+    <col min="2" max="2" width="63.109375" style="3" customWidth="1"/>
+    <col min="3" max="3" width="37.6640625" style="1" customWidth="1"/>
+    <col min="4" max="16384" width="8.88671875" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="20.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="145" t="s">
+      <c r="A1" s="146" t="s">
         <v>8</v>
       </c>
-      <c r="B1" s="145"/>
-      <c r="C1" s="145"/>
-      <c r="D1" s="145"/>
-      <c r="E1" s="145"/>
-      <c r="F1" s="145"/>
+      <c r="B1" s="146"/>
+      <c r="C1" s="146"/>
+      <c r="D1" s="146"/>
+      <c r="E1" s="146"/>
+      <c r="F1" s="146"/>
     </row>
     <row r="2" spans="1:6" ht="41.25" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="146" t="s">
+      <c r="A2" s="147" t="s">
         <v>68</v>
       </c>
-      <c r="B2" s="146"/>
+      <c r="B2" s="147"/>
       <c r="C2" s="2"/>
       <c r="D2" s="2"/>
       <c r="E2" s="2"/>
       <c r="F2" s="2"/>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A4" s="109" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="B4" s="114"/>
       <c r="C4" s="103"/>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A5" s="104" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="B5" s="107"/>
       <c r="C5" s="103"/>
     </row>
     <row r="6" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="104" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="B6" s="106"/>
       <c r="C6" s="103"/>
     </row>
     <row r="7" spans="1:6" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="111" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="B7" s="105"/>
       <c r="C7" s="115" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+      <c r="A8" s="111" t="s">
         <v>179</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A8" s="111" t="s">
-        <v>180</v>
       </c>
       <c r="B8" s="110"/>
       <c r="C8" s="113"/>
     </row>
     <row r="9" spans="1:6" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="111" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="B9" s="108"/>
       <c r="C9" s="116"/>
     </row>
     <row r="10" spans="1:6" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="111" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="B10" s="105"/>
       <c r="C10" s="115" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
     </row>
     <row r="11" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="111" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="B11" s="108"/>
       <c r="C11" s="116"/>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A12" s="104" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="B12" s="112"/>
       <c r="C12" s="103"/>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A13" s="104" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="B13" s="104"/>
       <c r="C13" s="103"/>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A14" s="104" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="B14" s="104"/>
       <c r="C14" s="103"/>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A15" s="104" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="B15" s="104"/>
       <c r="C15" s="103"/>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A16" s="104" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="B16" s="104"/>
       <c r="C16" s="103"/>
     </row>
-    <row r="17" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A17" s="104" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="B17" s="104"/>
       <c r="C17" s="103"/>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A18" s="104" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="B18" s="104"/>
       <c r="C18" s="80"/>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A19" s="104" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="B19" s="104"/>
       <c r="C19" s="80"/>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A20" s="104" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="B20" s="104"/>
       <c r="C20" s="80"/>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A21" s="104" t="s">
         <v>9</v>
       </c>
       <c r="B21" s="104"/>
       <c r="C21" s="80"/>
     </row>
-    <row r="22" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A22" s="104" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="B22" s="104"/>
       <c r="C22" s="80"/>
@@ -3990,38 +4013,38 @@
       <selection activeCell="A26" sqref="A26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="80.28515625" style="125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="26.5703125" style="125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="62.42578125" style="125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.28515625" style="125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="80.33203125" style="125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="26.5546875" style="125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="62.44140625" style="125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.33203125" style="125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="12" style="125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="5.85546875" style="125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="12.42578125" style="125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="17.42578125" style="125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="9.7109375" style="125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="10.7109375" style="125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="14.5703125" style="125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="35.5703125" style="125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="5.88671875" style="125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12.44140625" style="125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="17.44140625" style="125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="9.6640625" style="125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="10.6640625" style="125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="14.5546875" style="125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="35.5546875" style="125" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="10" style="128" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="5.42578125" style="125" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="9.5703125" style="125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="5.44140625" style="125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="9.5546875" style="125" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="11" style="126" bestFit="1" customWidth="1"/>
     <col min="17" max="17" width="10" style="125" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="26.5703125" style="125" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="26.5546875" style="125" bestFit="1" customWidth="1"/>
     <col min="19" max="19" width="19" style="125" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="16.42578125" style="128" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="16.140625" style="128" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="10.42578125" style="125" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="12.7109375" style="125" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="21.28515625" style="125" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="19.140625" style="129" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="19.5703125" style="129" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="217.28515625" style="125" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="11.7109375" style="125" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="16.42578125" style="125" bestFit="1" customWidth="1"/>
-    <col min="30" max="16384" width="9.140625" style="125"/>
+    <col min="20" max="20" width="16.44140625" style="128" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="16.109375" style="128" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="10.44140625" style="125" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="12.6640625" style="125" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="21.33203125" style="125" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="19.109375" style="129" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="19.5546875" style="129" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="217.33203125" style="125" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="11.6640625" style="125" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="16.44140625" style="125" bestFit="1" customWidth="1"/>
+    <col min="30" max="16384" width="9.109375" style="125"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:29" s="120" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -4115,13 +4138,13 @@
     </row>
     <row r="2" spans="1:29" s="117" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="79" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="B2" s="121" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="C2" s="121" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="D2" s="121" t="s">
         <v>14</v>
@@ -4130,10 +4153,10 @@
         <v>20</v>
       </c>
       <c r="G2" s="121" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="H2" s="122" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="I2" s="123">
         <v>532397.91460000002</v>
@@ -4142,16 +4165,16 @@
         <v>4489414.8002500003</v>
       </c>
       <c r="K2" s="78" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="L2" s="117" t="s">
+        <v>136</v>
+      </c>
+      <c r="M2" s="78" t="s">
         <v>137</v>
       </c>
-      <c r="M2" s="78" t="s">
-        <v>138</v>
-      </c>
       <c r="N2" s="121" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="O2" s="124">
         <v>40.554862</v>
@@ -4160,13 +4183,13 @@
         <v>-116.617339</v>
       </c>
       <c r="Q2" s="78" t="s">
+        <v>133</v>
+      </c>
+      <c r="R2" s="78" t="s">
         <v>134</v>
       </c>
-      <c r="R2" s="78" t="s">
-        <v>135</v>
-      </c>
       <c r="S2" s="139" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="T2" s="77">
         <v>40148</v>
@@ -4184,33 +4207,33 @@
         <v>9551</v>
       </c>
       <c r="AA2" s="121" t="s">
+        <v>139</v>
+      </c>
+      <c r="AC2" s="117" t="s">
         <v>140</v>
-      </c>
-      <c r="AC2" s="117" t="s">
-        <v>141</v>
       </c>
     </row>
     <row r="3" spans="1:29" s="117" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="79" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="B3" s="121" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="C3" s="121" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="D3" s="121" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="E3" s="121" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="G3" s="121" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="H3" s="122" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="I3" s="123">
         <v>261800.44073</v>
@@ -4219,16 +4242,16 @@
         <v>4361795.6038899999</v>
       </c>
       <c r="K3" s="78" t="s">
+        <v>128</v>
+      </c>
+      <c r="L3" s="117" t="s">
+        <v>141</v>
+      </c>
+      <c r="M3" s="78" t="s">
         <v>129</v>
       </c>
-      <c r="L3" s="117" t="s">
-        <v>142</v>
-      </c>
-      <c r="M3" s="78" t="s">
-        <v>130</v>
-      </c>
       <c r="N3" s="121" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="O3" s="124">
         <v>39.372798000000003</v>
@@ -4237,13 +4260,13 @@
         <v>-119.765193</v>
       </c>
       <c r="Q3" s="78" t="s">
+        <v>133</v>
+      </c>
+      <c r="R3" s="78" t="s">
         <v>134</v>
       </c>
-      <c r="R3" s="78" t="s">
-        <v>135</v>
-      </c>
       <c r="S3" s="139" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="T3" s="77">
         <v>39203</v>
@@ -4261,21 +4284,21 @@
         <v>6445.74</v>
       </c>
       <c r="AA3" s="121" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="AC3" s="117" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
     </row>
     <row r="4" spans="1:29" s="117" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="79" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="B4" s="121" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="C4" s="121" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="D4" s="121" t="s">
         <v>42</v>
@@ -4284,10 +4307,10 @@
         <v>44</v>
       </c>
       <c r="G4" s="121" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="H4" s="77" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="I4" s="123">
         <v>366228.27308000001</v>
@@ -4296,16 +4319,16 @@
         <v>4378732.2786400001</v>
       </c>
       <c r="K4" s="78" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="L4" s="117" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="M4" s="78" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="N4" s="121" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="O4" s="124">
         <v>39.547848999999999</v>
@@ -4314,13 +4337,13 @@
         <v>-118.55689599999999</v>
       </c>
       <c r="Q4" s="78" t="s">
+        <v>133</v>
+      </c>
+      <c r="R4" s="78" t="s">
         <v>134</v>
       </c>
-      <c r="R4" s="78" t="s">
-        <v>135</v>
-      </c>
       <c r="S4" s="139" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="T4" s="77">
         <v>36495</v>
@@ -4338,33 +4361,33 @@
         <v>7540.8</v>
       </c>
       <c r="AA4" s="121" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="AC4" s="117" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
     </row>
     <row r="5" spans="1:29" s="117" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="79" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="B5" s="121" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="C5" s="121" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="D5" s="121" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="E5" s="121" t="s">
         <v>43</v>
       </c>
       <c r="G5" s="121" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="H5" s="122" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="I5" s="123">
         <v>341112.44394999999</v>
@@ -4373,16 +4396,16 @@
         <v>4380170.5932299998</v>
       </c>
       <c r="K5" s="78" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="L5" s="117" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="M5" s="117" t="s">
+        <v>131</v>
+      </c>
+      <c r="N5" s="121" t="s">
         <v>132</v>
-      </c>
-      <c r="N5" s="121" t="s">
-        <v>133</v>
       </c>
       <c r="O5" s="124">
         <v>39.556520999999996</v>
@@ -4391,13 +4414,13 @@
         <v>-118.849418</v>
       </c>
       <c r="Q5" s="78" t="s">
+        <v>133</v>
+      </c>
+      <c r="R5" s="78" t="s">
         <v>134</v>
       </c>
-      <c r="R5" s="78" t="s">
-        <v>135</v>
-      </c>
       <c r="S5" s="139" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="T5" s="77">
         <v>36861</v>
@@ -4415,10 +4438,10 @@
         <v>7543.2</v>
       </c>
       <c r="AA5" s="121" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="AC5" s="117" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
     </row>
     <row r="6" spans="1:29" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -4456,7 +4479,7 @@
       <c r="Y8" s="125"/>
       <c r="Z8" s="125"/>
     </row>
-    <row r="9" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:29" ht="15" x14ac:dyDescent="0.25">
       <c r="C9" s="126"/>
       <c r="D9" s="143"/>
       <c r="I9" s="127"/>
@@ -4467,7 +4490,7 @@
       <c r="Y9" s="125"/>
       <c r="Z9" s="125"/>
     </row>
-    <row r="10" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:29" ht="15" x14ac:dyDescent="0.25">
       <c r="C10" s="126"/>
       <c r="D10" s="143"/>
       <c r="I10" s="127"/>
@@ -4478,7 +4501,7 @@
       <c r="Y10" s="125"/>
       <c r="Z10" s="125"/>
     </row>
-    <row r="11" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:29" ht="15" x14ac:dyDescent="0.25">
       <c r="C11" s="126"/>
       <c r="D11" s="143"/>
       <c r="I11" s="127"/>
@@ -4489,7 +4512,7 @@
       <c r="Y11" s="125"/>
       <c r="Z11" s="125"/>
     </row>
-    <row r="12" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:29" ht="15" x14ac:dyDescent="0.25">
       <c r="C12" s="126"/>
       <c r="D12" s="143"/>
       <c r="I12" s="127"/>
@@ -4500,7 +4523,7 @@
       <c r="Y12" s="125"/>
       <c r="Z12" s="125"/>
     </row>
-    <row r="13" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:29" ht="15" x14ac:dyDescent="0.25">
       <c r="C13" s="126"/>
       <c r="D13" s="143"/>
       <c r="I13" s="127"/>
@@ -4511,7 +4534,7 @@
       <c r="Y13" s="125"/>
       <c r="Z13" s="125"/>
     </row>
-    <row r="14" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:29" ht="15" x14ac:dyDescent="0.25">
       <c r="C14" s="144"/>
       <c r="D14" s="144"/>
       <c r="I14" s="127"/>
@@ -4522,7 +4545,7 @@
       <c r="Y14" s="125"/>
       <c r="Z14" s="125"/>
     </row>
-    <row r="15" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:29" ht="15" x14ac:dyDescent="0.25">
       <c r="C15" s="144"/>
       <c r="D15" s="144"/>
       <c r="I15" s="127"/>
@@ -4533,7 +4556,7 @@
       <c r="Y15" s="125"/>
       <c r="Z15" s="125"/>
     </row>
-    <row r="16" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:29" ht="15" x14ac:dyDescent="0.25">
       <c r="C16" s="126"/>
       <c r="D16" s="143"/>
       <c r="I16" s="127"/>
@@ -4544,7 +4567,7 @@
       <c r="Y16" s="125"/>
       <c r="Z16" s="125"/>
     </row>
-    <row r="17" spans="3:21" s="125" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="3:21" s="125" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="C17" s="126"/>
       <c r="D17" s="143"/>
       <c r="I17" s="127"/>
@@ -4553,7 +4576,7 @@
       <c r="T17" s="128"/>
       <c r="U17" s="128"/>
     </row>
-    <row r="18" spans="3:21" s="125" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="3:21" s="125" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="C18" s="126"/>
       <c r="D18" s="143"/>
       <c r="I18" s="127"/>
@@ -4562,7 +4585,7 @@
       <c r="T18" s="128"/>
       <c r="U18" s="128"/>
     </row>
-    <row r="19" spans="3:21" s="125" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="3:21" s="125" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="C19" s="126"/>
       <c r="D19" s="143"/>
       <c r="I19" s="127"/>
@@ -4571,7 +4594,7 @@
       <c r="T19" s="128"/>
       <c r="U19" s="128"/>
     </row>
-    <row r="20" spans="3:21" s="125" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="3:21" s="125" customFormat="1" x14ac:dyDescent="0.3">
       <c r="C20" s="126"/>
       <c r="D20" s="143"/>
       <c r="I20" s="127"/>
@@ -4580,7 +4603,7 @@
       <c r="T20" s="128"/>
       <c r="U20" s="128"/>
     </row>
-    <row r="21" spans="3:21" s="125" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="3:21" s="125" customFormat="1" x14ac:dyDescent="0.3">
       <c r="C21" s="144"/>
       <c r="D21" s="144"/>
       <c r="I21" s="127"/>
@@ -4589,7 +4612,7 @@
       <c r="T21" s="128"/>
       <c r="U21" s="128"/>
     </row>
-    <row r="22" spans="3:21" s="125" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="3:21" s="125" customFormat="1" x14ac:dyDescent="0.3">
       <c r="C22" s="126"/>
       <c r="D22" s="143"/>
       <c r="I22" s="127"/>
@@ -4598,14 +4621,14 @@
       <c r="T22" s="128"/>
       <c r="U22" s="128"/>
     </row>
-    <row r="23" spans="3:21" s="125" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="3:21" s="125" customFormat="1" x14ac:dyDescent="0.3">
       <c r="C23" s="126"/>
       <c r="D23" s="143"/>
       <c r="N23" s="127"/>
       <c r="T23" s="128"/>
       <c r="U23" s="128"/>
     </row>
-    <row r="24" spans="3:21" s="125" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="3:21" s="125" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C24" s="126"/>
       <c r="D24" s="143"/>
       <c r="I24" s="127"/>
@@ -4614,7 +4637,7 @@
       <c r="T24" s="128"/>
       <c r="U24" s="128"/>
     </row>
-    <row r="25" spans="3:21" s="125" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="3:21" s="125" customFormat="1" x14ac:dyDescent="0.3">
       <c r="C25" s="126"/>
       <c r="D25" s="143"/>
       <c r="I25" s="127"/>
@@ -4623,7 +4646,7 @@
       <c r="T25" s="128"/>
       <c r="U25" s="128"/>
     </row>
-    <row r="26" spans="3:21" s="125" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="3:21" s="125" customFormat="1" x14ac:dyDescent="0.3">
       <c r="C26" s="126"/>
       <c r="D26" s="143"/>
       <c r="I26" s="127"/>
@@ -4632,7 +4655,7 @@
       <c r="T26" s="128"/>
       <c r="U26" s="128"/>
     </row>
-    <row r="27" spans="3:21" s="125" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="3:21" s="125" customFormat="1" x14ac:dyDescent="0.3">
       <c r="C27" s="126"/>
       <c r="D27" s="143"/>
       <c r="I27" s="127"/>
@@ -4641,7 +4664,7 @@
       <c r="T27" s="128"/>
       <c r="U27" s="128"/>
     </row>
-    <row r="28" spans="3:21" s="125" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="3:21" s="125" customFormat="1" x14ac:dyDescent="0.3">
       <c r="C28" s="126"/>
       <c r="D28" s="143"/>
       <c r="I28" s="127"/>
@@ -4650,7 +4673,7 @@
       <c r="T28" s="128"/>
       <c r="U28" s="128"/>
     </row>
-    <row r="29" spans="3:21" s="125" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="3:21" s="125" customFormat="1" x14ac:dyDescent="0.3">
       <c r="C29" s="126"/>
       <c r="D29" s="143"/>
       <c r="I29" s="127"/>
@@ -4659,7 +4682,7 @@
       <c r="T29" s="128"/>
       <c r="U29" s="128"/>
     </row>
-    <row r="30" spans="3:21" s="125" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="3:21" s="125" customFormat="1" x14ac:dyDescent="0.3">
       <c r="C30" s="144"/>
       <c r="D30" s="144"/>
       <c r="I30" s="127"/>
@@ -4668,7 +4691,7 @@
       <c r="T30" s="128"/>
       <c r="U30" s="128"/>
     </row>
-    <row r="31" spans="3:21" s="125" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="3:21" s="125" customFormat="1" x14ac:dyDescent="0.3">
       <c r="C31" s="144"/>
       <c r="D31" s="144"/>
       <c r="I31" s="127"/>
@@ -4677,7 +4700,7 @@
       <c r="T31" s="128"/>
       <c r="U31" s="128"/>
     </row>
-    <row r="32" spans="3:21" s="125" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="3:21" s="125" customFormat="1" x14ac:dyDescent="0.3">
       <c r="C32" s="126"/>
       <c r="D32" s="143"/>
       <c r="I32" s="127"/>
@@ -4686,7 +4709,7 @@
       <c r="T32" s="128"/>
       <c r="U32" s="128"/>
     </row>
-    <row r="33" spans="3:21" s="125" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="3:21" s="125" customFormat="1" x14ac:dyDescent="0.3">
       <c r="C33" s="126"/>
       <c r="D33" s="143"/>
       <c r="I33" s="127"/>
@@ -4695,7 +4718,7 @@
       <c r="T33" s="128"/>
       <c r="U33" s="128"/>
     </row>
-    <row r="34" spans="3:21" s="125" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="3:21" s="125" customFormat="1" x14ac:dyDescent="0.3">
       <c r="C34" s="126"/>
       <c r="D34" s="143"/>
       <c r="I34" s="127"/>
@@ -4704,7 +4727,7 @@
       <c r="T34" s="128"/>
       <c r="U34" s="128"/>
     </row>
-    <row r="35" spans="3:21" s="125" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="3:21" s="125" customFormat="1" x14ac:dyDescent="0.3">
       <c r="C35" s="126"/>
       <c r="D35" s="143"/>
       <c r="I35" s="127"/>
@@ -4713,7 +4736,7 @@
       <c r="T35" s="128"/>
       <c r="U35" s="128"/>
     </row>
-    <row r="36" spans="3:21" s="125" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="3:21" s="125" customFormat="1" x14ac:dyDescent="0.3">
       <c r="C36" s="126"/>
       <c r="D36" s="143"/>
       <c r="I36" s="127"/>
@@ -4722,7 +4745,7 @@
       <c r="T36" s="128"/>
       <c r="U36" s="128"/>
     </row>
-    <row r="37" spans="3:21" s="125" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="3:21" s="125" customFormat="1" x14ac:dyDescent="0.3">
       <c r="C37" s="144"/>
       <c r="D37" s="144"/>
       <c r="I37" s="127"/>
@@ -4731,7 +4754,7 @@
       <c r="T37" s="128"/>
       <c r="U37" s="128"/>
     </row>
-    <row r="38" spans="3:21" s="125" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="3:21" s="125" customFormat="1" x14ac:dyDescent="0.3">
       <c r="C38" s="126"/>
       <c r="D38" s="143"/>
       <c r="I38" s="127"/>
@@ -4740,66 +4763,66 @@
       <c r="T38" s="128"/>
       <c r="U38" s="128"/>
     </row>
-    <row r="39" spans="3:21" s="125" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="3:21" s="125" customFormat="1" x14ac:dyDescent="0.3">
       <c r="C39" s="126"/>
       <c r="D39" s="143"/>
       <c r="N39" s="127"/>
       <c r="T39" s="128"/>
       <c r="U39" s="128"/>
     </row>
-    <row r="40" spans="3:21" s="125" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="40" spans="3:21" s="125" customFormat="1" x14ac:dyDescent="0.3">
       <c r="T40" s="128"/>
       <c r="U40" s="128"/>
     </row>
-    <row r="41" spans="3:21" s="125" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="41" spans="3:21" s="125" customFormat="1" x14ac:dyDescent="0.3">
       <c r="T41" s="128"/>
       <c r="U41" s="128"/>
     </row>
-    <row r="42" spans="3:21" s="125" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="42" spans="3:21" s="125" customFormat="1" x14ac:dyDescent="0.3">
       <c r="T42" s="128"/>
       <c r="U42" s="128"/>
     </row>
-    <row r="43" spans="3:21" s="125" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="43" spans="3:21" s="125" customFormat="1" x14ac:dyDescent="0.3">
       <c r="T43" s="128"/>
       <c r="U43" s="128"/>
     </row>
-    <row r="44" spans="3:21" s="125" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="44" spans="3:21" s="125" customFormat="1" x14ac:dyDescent="0.3">
       <c r="T44" s="128"/>
       <c r="U44" s="128"/>
     </row>
-    <row r="45" spans="3:21" s="125" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="45" spans="3:21" s="125" customFormat="1" x14ac:dyDescent="0.3">
       <c r="T45" s="128"/>
       <c r="U45" s="128"/>
     </row>
-    <row r="46" spans="3:21" s="125" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="46" spans="3:21" s="125" customFormat="1" x14ac:dyDescent="0.3">
       <c r="T46" s="128"/>
       <c r="U46" s="128"/>
     </row>
-    <row r="47" spans="3:21" s="125" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="47" spans="3:21" s="125" customFormat="1" x14ac:dyDescent="0.3">
       <c r="T47" s="128"/>
       <c r="U47" s="128"/>
     </row>
-    <row r="48" spans="3:21" s="125" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="48" spans="3:21" s="125" customFormat="1" x14ac:dyDescent="0.3">
       <c r="T48" s="128"/>
       <c r="U48" s="128"/>
     </row>
-    <row r="49" spans="20:21" s="125" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="49" spans="20:21" s="125" customFormat="1" x14ac:dyDescent="0.3">
       <c r="T49" s="128"/>
       <c r="U49" s="128"/>
     </row>
-    <row r="50" spans="20:21" s="125" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="50" spans="20:21" s="125" customFormat="1" x14ac:dyDescent="0.3">
       <c r="T50" s="128"/>
       <c r="U50" s="128"/>
     </row>
-    <row r="51" spans="20:21" s="125" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="51" spans="20:21" s="125" customFormat="1" x14ac:dyDescent="0.3">
       <c r="T51" s="128"/>
       <c r="U51" s="128"/>
     </row>
-    <row r="52" spans="20:21" s="125" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="52" spans="20:21" s="125" customFormat="1" x14ac:dyDescent="0.3">
       <c r="T52" s="128"/>
       <c r="U52" s="128"/>
     </row>
-    <row r="53" spans="20:21" s="125" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="53" spans="20:21" s="125" customFormat="1" x14ac:dyDescent="0.3">
       <c r="T53" s="128"/>
       <c r="U53" s="128"/>
     </row>
@@ -4827,30 +4850,30 @@
   </sheetPr>
   <dimension ref="A1:BJ34"/>
   <sheetViews>
-    <sheetView topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="C43" sqref="C43"/>
+    <sheetView topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="A27" sqref="A27:A30"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="14.25" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="13.8" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="25.7109375" style="11" customWidth="1"/>
-    <col min="2" max="2" width="18.7109375" style="14" customWidth="1"/>
+    <col min="1" max="1" width="25.6640625" style="11" customWidth="1"/>
+    <col min="2" max="2" width="18.6640625" style="14" customWidth="1"/>
     <col min="3" max="3" width="21" style="14" customWidth="1"/>
-    <col min="4" max="4" width="15.85546875" style="14" customWidth="1"/>
-    <col min="5" max="5" width="46.85546875" style="14" customWidth="1"/>
-    <col min="6" max="6" width="39.140625" style="14" customWidth="1"/>
-    <col min="7" max="7" width="40.85546875" style="14" customWidth="1"/>
-    <col min="8" max="16384" width="9.140625" style="15"/>
+    <col min="4" max="4" width="15.88671875" style="14" customWidth="1"/>
+    <col min="5" max="5" width="46.88671875" style="14" customWidth="1"/>
+    <col min="6" max="6" width="39.109375" style="14" customWidth="1"/>
+    <col min="7" max="7" width="40.88671875" style="14" customWidth="1"/>
+    <col min="8" max="16384" width="9.109375" style="15"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:62" s="11" customFormat="1" ht="19.5" x14ac:dyDescent="0.25">
-      <c r="A1" s="147" t="s">
+      <c r="A1" s="148" t="s">
         <v>21</v>
       </c>
-      <c r="B1" s="147"/>
-      <c r="C1" s="147"/>
-      <c r="D1" s="147"/>
-      <c r="E1" s="147"/>
+      <c r="B1" s="148"/>
+      <c r="C1" s="148"/>
+      <c r="D1" s="148"/>
+      <c r="E1" s="148"/>
       <c r="F1" s="9"/>
       <c r="G1" s="9"/>
       <c r="H1" s="10"/>
@@ -4910,13 +4933,13 @@
       <c r="BJ1" s="10"/>
     </row>
     <row r="2" spans="1:62" s="11" customFormat="1" ht="53.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="148" t="s">
+      <c r="A2" s="149" t="s">
         <v>22</v>
       </c>
-      <c r="B2" s="148"/>
-      <c r="C2" s="148"/>
-      <c r="D2" s="148"/>
-      <c r="E2" s="148"/>
+      <c r="B2" s="149"/>
+      <c r="C2" s="149"/>
+      <c r="D2" s="149"/>
+      <c r="E2" s="149"/>
       <c r="F2" s="12"/>
       <c r="G2" s="12"/>
       <c r="H2" s="10"/>
@@ -5291,7 +5314,7 @@
       <c r="F10" s="28"/>
       <c r="G10" s="23"/>
     </row>
-    <row r="11" spans="1:62" s="6" customFormat="1" ht="35.450000000000003" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:62" s="6" customFormat="1" ht="35.4" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="8" t="s">
         <v>47</v>
       </c>
@@ -5310,21 +5333,21 @@
       <c r="F11" s="28"/>
       <c r="G11" s="23"/>
     </row>
-    <row r="12" spans="1:62" s="6" customFormat="1" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:62" s="6" customFormat="1" ht="39.6" x14ac:dyDescent="0.3">
       <c r="A12" s="8" t="s">
         <v>69</v>
       </c>
       <c r="B12" s="37" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C12" s="37" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="D12" s="37" t="s">
         <v>35</v>
       </c>
       <c r="E12" s="37" t="s">
-        <v>100</v>
+        <v>199</v>
       </c>
       <c r="F12" s="23"/>
       <c r="G12" s="23"/>
@@ -5343,7 +5366,7 @@
         <v>35</v>
       </c>
       <c r="E13" s="37" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="F13" s="23"/>
       <c r="G13" s="23"/>
@@ -5519,7 +5542,7 @@
       <c r="F22" s="24"/>
       <c r="G22" s="24"/>
     </row>
-    <row r="23" spans="1:11" s="6" customFormat="1" ht="31.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:11" s="6" customFormat="1" ht="31.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="29" t="s">
         <v>72</v>
       </c>
@@ -5595,7 +5618,7 @@
       <c r="F26" s="23"/>
       <c r="G26" s="23"/>
     </row>
-    <row r="27" spans="1:11" s="6" customFormat="1" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:11" s="6" customFormat="1" ht="26.4" x14ac:dyDescent="0.3">
       <c r="A27" s="31" t="s">
         <v>16</v>
       </c>
@@ -5603,7 +5626,7 @@
         <v>36</v>
       </c>
       <c r="C27" s="38" t="s">
-        <v>33</v>
+        <v>50</v>
       </c>
       <c r="D27" s="40" t="s">
         <v>35</v>
@@ -5614,7 +5637,7 @@
       <c r="F27" s="23"/>
       <c r="G27" s="23"/>
     </row>
-    <row r="28" spans="1:11" s="6" customFormat="1" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:11" s="6" customFormat="1" ht="26.4" x14ac:dyDescent="0.3">
       <c r="A28" s="31" t="s">
         <v>82</v>
       </c>
@@ -5622,7 +5645,7 @@
         <v>36</v>
       </c>
       <c r="C28" s="38" t="s">
-        <v>33</v>
+        <v>50</v>
       </c>
       <c r="D28" s="41" t="s">
         <v>35</v>
@@ -5633,7 +5656,7 @@
       <c r="F28" s="23"/>
       <c r="G28" s="23"/>
     </row>
-    <row r="29" spans="1:11" s="6" customFormat="1" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:11" s="6" customFormat="1" ht="26.4" x14ac:dyDescent="0.3">
       <c r="A29" s="31" t="s">
         <v>83</v>
       </c>
@@ -5641,7 +5664,7 @@
         <v>36</v>
       </c>
       <c r="C29" s="38" t="s">
-        <v>33</v>
+        <v>50</v>
       </c>
       <c r="D29" s="41" t="s">
         <v>35</v>
@@ -5652,7 +5675,7 @@
       <c r="F29" s="23"/>
       <c r="G29" s="23"/>
     </row>
-    <row r="30" spans="1:11" s="6" customFormat="1" ht="38.25" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:11" s="6" customFormat="1" ht="39.6" x14ac:dyDescent="0.3">
       <c r="A30" s="31" t="s">
         <v>84</v>
       </c>
@@ -5660,7 +5683,7 @@
         <v>36</v>
       </c>
       <c r="C30" s="38" t="s">
-        <v>33</v>
+        <v>50</v>
       </c>
       <c r="D30" s="41" t="s">
         <v>35</v>
@@ -5690,7 +5713,7 @@
       <c r="F31" s="23"/>
       <c r="G31" s="23"/>
     </row>
-    <row r="32" spans="1:11" ht="38.25" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:11" ht="39.6" x14ac:dyDescent="0.3">
       <c r="A32" s="5" t="s">
         <v>12</v>
       </c>
@@ -5713,7 +5736,7 @@
       <c r="J32" s="6"/>
       <c r="K32" s="6"/>
     </row>
-    <row r="33" spans="1:10" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:10" ht="26.4" x14ac:dyDescent="0.3">
       <c r="A33" s="18" t="s">
         <v>38</v>
       </c>
@@ -5735,7 +5758,7 @@
       <c r="I33" s="6"/>
       <c r="J33" s="6"/>
     </row>
-    <row r="34" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A34" s="10"/>
       <c r="B34" s="17"/>
     </row>
@@ -5758,20 +5781,20 @@
       <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="9.140625" style="7"/>
+    <col min="1" max="1" width="9.109375" style="7"/>
     <col min="2" max="2" width="22" style="4" customWidth="1"/>
-    <col min="3" max="3" width="61.140625" style="4" customWidth="1"/>
-    <col min="4" max="4" width="55.42578125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="43.140625" customWidth="1"/>
+    <col min="3" max="3" width="61.109375" style="4" customWidth="1"/>
+    <col min="4" max="4" width="55.44140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="43.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="B1"/>
       <c r="C1"/>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="A2" s="51" t="s">
         <v>64</v>
       </c>
@@ -5784,68 +5807,68 @@
     <row r="3" spans="1:5" ht="60" x14ac:dyDescent="0.25">
       <c r="A3" s="52"/>
       <c r="B3" s="52" t="s">
+        <v>105</v>
+      </c>
+      <c r="C3" s="48" t="s">
+        <v>107</v>
+      </c>
+      <c r="D3" s="49" t="s">
         <v>106</v>
       </c>
-      <c r="C3" s="48" t="s">
-        <v>108</v>
-      </c>
-      <c r="D3" s="49" t="s">
-        <v>107</v>
-      </c>
       <c r="E3" s="46"/>
     </row>
-    <row r="4" spans="1:5" ht="75" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A4" s="52"/>
       <c r="B4" s="52" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C4" s="50" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="D4" s="49" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="E4" s="46"/>
     </row>
     <row r="5" spans="1:5" ht="75" x14ac:dyDescent="0.25">
       <c r="A5" s="52"/>
       <c r="B5" s="52" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="C5" s="50" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="D5" s="49" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="E5" s="46"/>
     </row>
     <row r="6" spans="1:5" ht="60" x14ac:dyDescent="0.25">
       <c r="A6" s="52"/>
       <c r="B6" s="52" t="s">
+        <v>112</v>
+      </c>
+      <c r="C6" s="50" t="s">
         <v>113</v>
       </c>
-      <c r="C6" s="50" t="s">
-        <v>114</v>
-      </c>
       <c r="D6" s="49" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="E6" s="46"/>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B7"/>
       <c r="C7"/>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B8"/>
       <c r="C8"/>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B9"/>
       <c r="C9"/>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B10"/>
       <c r="C10"/>
     </row>
@@ -5869,18 +5892,18 @@
       <selection activeCell="D22" sqref="D22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="18.5703125" customWidth="1"/>
-    <col min="2" max="2" width="11.42578125" customWidth="1"/>
-    <col min="3" max="3" width="24.7109375" customWidth="1"/>
-    <col min="4" max="4" width="53.140625" customWidth="1"/>
-    <col min="5" max="9" width="16.140625" customWidth="1"/>
+    <col min="1" max="1" width="18.5546875" customWidth="1"/>
+    <col min="2" max="2" width="11.44140625" customWidth="1"/>
+    <col min="3" max="3" width="24.6640625" customWidth="1"/>
+    <col min="4" max="4" width="53.109375" customWidth="1"/>
+    <col min="5" max="9" width="16.109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A1" s="84" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="B1" s="80"/>
       <c r="C1" s="80"/>
@@ -5907,13 +5930,13 @@
       <c r="K2" s="80"/>
     </row>
     <row r="3" spans="1:11" ht="41.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="150" t="s">
-        <v>158</v>
-      </c>
-      <c r="B3" s="150"/>
-      <c r="C3" s="150"/>
-      <c r="D3" s="150"/>
-      <c r="E3" s="150"/>
+      <c r="A3" s="151" t="s">
+        <v>157</v>
+      </c>
+      <c r="B3" s="151"/>
+      <c r="C3" s="151"/>
+      <c r="D3" s="151"/>
+      <c r="E3" s="151"/>
       <c r="F3" s="80"/>
       <c r="G3" s="80"/>
       <c r="H3" s="80"/>
@@ -5935,15 +5958,15 @@
       <c r="K4" s="80"/>
     </row>
     <row r="5" spans="1:11" ht="70.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="154" t="s">
-        <v>159</v>
-      </c>
-      <c r="B5" s="155"/>
-      <c r="C5" s="155"/>
-      <c r="D5" s="155"/>
-      <c r="E5" s="155"/>
-      <c r="F5" s="155"/>
-      <c r="G5" s="156"/>
+      <c r="A5" s="155" t="s">
+        <v>158</v>
+      </c>
+      <c r="B5" s="156"/>
+      <c r="C5" s="156"/>
+      <c r="D5" s="156"/>
+      <c r="E5" s="156"/>
+      <c r="F5" s="156"/>
+      <c r="G5" s="157"/>
       <c r="H5" s="80"/>
       <c r="I5" s="80"/>
       <c r="J5" s="80"/>
@@ -5963,12 +5986,12 @@
       <c r="K6" s="80"/>
     </row>
     <row r="7" spans="1:11" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="151" t="s">
-        <v>160</v>
-      </c>
-      <c r="B7" s="152"/>
-      <c r="C7" s="152"/>
-      <c r="D7" s="153"/>
+      <c r="A7" s="152" t="s">
+        <v>159</v>
+      </c>
+      <c r="B7" s="153"/>
+      <c r="C7" s="153"/>
+      <c r="D7" s="154"/>
       <c r="E7" s="80"/>
       <c r="F7" s="80"/>
       <c r="G7" s="80"/>
@@ -5992,7 +6015,7 @@
     </row>
     <row r="9" spans="1:11" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A9" s="87" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="B9" s="80"/>
       <c r="C9" s="80"/>
@@ -6006,10 +6029,10 @@
       <c r="K9" s="80"/>
     </row>
     <row r="10" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="149"/>
-      <c r="B10" s="149"/>
-      <c r="C10" s="149"/>
-      <c r="D10" s="149"/>
+      <c r="A10" s="150"/>
+      <c r="B10" s="150"/>
+      <c r="C10" s="150"/>
+      <c r="D10" s="150"/>
       <c r="E10" s="81"/>
       <c r="F10" s="81"/>
       <c r="G10" s="80"/>
@@ -6020,28 +6043,28 @@
     </row>
     <row r="11" spans="1:11" ht="32.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="96" t="s">
+        <v>161</v>
+      </c>
+      <c r="B11" s="96" t="s">
         <v>162</v>
       </c>
-      <c r="B11" s="96" t="s">
+      <c r="C11" s="96" t="s">
         <v>163</v>
-      </c>
-      <c r="C11" s="96" t="s">
-        <v>164</v>
       </c>
       <c r="D11" s="96" t="s">
         <v>5</v>
       </c>
       <c r="E11" s="96" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="F11" s="99" t="s">
         <v>7</v>
       </c>
       <c r="G11" s="96" t="s">
+        <v>165</v>
+      </c>
+      <c r="H11" s="96" t="s">
         <v>166</v>
-      </c>
-      <c r="H11" s="96" t="s">
-        <v>167</v>
       </c>
       <c r="I11" s="99" t="s">
         <v>7</v>
@@ -6049,7 +6072,7 @@
       <c r="J11" s="80"/>
       <c r="K11" s="80"/>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:11" ht="15" x14ac:dyDescent="0.25">
       <c r="A12" s="95"/>
       <c r="B12" s="95"/>
       <c r="C12" s="86"/>
@@ -6067,19 +6090,19 @@
       <c r="B13" s="95"/>
       <c r="C13" s="95"/>
       <c r="D13" s="92" t="s">
+        <v>167</v>
+      </c>
+      <c r="E13" s="92" t="s">
         <v>168</v>
-      </c>
-      <c r="E13" s="92" t="s">
-        <v>169</v>
       </c>
       <c r="F13" s="91">
         <v>40766</v>
       </c>
       <c r="G13" s="90" t="s">
+        <v>169</v>
+      </c>
+      <c r="H13" s="92" t="s">
         <v>170</v>
-      </c>
-      <c r="H13" s="92" t="s">
-        <v>171</v>
       </c>
       <c r="I13" s="82">
         <v>40770</v>
@@ -6092,7 +6115,7 @@
       <c r="B14" s="93"/>
       <c r="C14" s="93"/>
       <c r="D14" s="92" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="E14" s="92"/>
       <c r="F14" s="89"/>
@@ -6102,7 +6125,7 @@
       <c r="J14" s="80"/>
       <c r="K14" s="80"/>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:11" ht="15" x14ac:dyDescent="0.25">
       <c r="A15" s="95"/>
       <c r="B15" s="93"/>
       <c r="C15" s="93"/>
@@ -6120,7 +6143,7 @@
       <c r="B16" s="93"/>
       <c r="C16" s="93"/>
       <c r="D16" s="100" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="E16" s="95"/>
       <c r="F16" s="94"/>
@@ -6130,7 +6153,7 @@
       <c r="J16" s="80"/>
       <c r="K16" s="80"/>
     </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:11" ht="15" x14ac:dyDescent="0.25">
       <c r="A17" s="95"/>
       <c r="B17" s="93"/>
       <c r="C17" s="93"/>
@@ -6143,7 +6166,7 @@
       <c r="J17" s="80"/>
       <c r="K17" s="80"/>
     </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:11" ht="15" x14ac:dyDescent="0.25">
       <c r="A18" s="95"/>
       <c r="B18" s="93"/>
       <c r="C18" s="93"/>
@@ -6156,7 +6179,7 @@
       <c r="J18" s="80"/>
       <c r="K18" s="102"/>
     </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:11" ht="15" x14ac:dyDescent="0.25">
       <c r="A19" s="95"/>
       <c r="B19" s="93"/>
       <c r="C19" s="93"/>
@@ -6169,7 +6192,7 @@
       <c r="J19" s="80"/>
       <c r="K19" s="80"/>
     </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:11" ht="15" x14ac:dyDescent="0.25">
       <c r="A20" s="83"/>
       <c r="B20" s="93"/>
       <c r="C20" s="93"/>
@@ -6182,7 +6205,7 @@
       <c r="J20" s="80"/>
       <c r="K20" s="80"/>
     </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A21" s="95"/>
       <c r="B21" s="93"/>
       <c r="C21" s="93"/>
@@ -6195,7 +6218,7 @@
       <c r="J21" s="80"/>
       <c r="K21" s="80"/>
     </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A22" s="95"/>
       <c r="B22" s="93"/>
       <c r="C22" s="93"/>
@@ -6208,7 +6231,7 @@
       <c r="J22" s="80"/>
       <c r="K22" s="80"/>
     </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A23" s="95"/>
       <c r="B23" s="93"/>
       <c r="C23" s="93"/>
@@ -6221,7 +6244,7 @@
       <c r="J23" s="80"/>
       <c r="K23" s="80"/>
     </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A24" s="95"/>
       <c r="B24" s="93"/>
       <c r="C24" s="93"/>
@@ -6234,7 +6257,7 @@
       <c r="J24" s="80"/>
       <c r="K24" s="80"/>
     </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A25" s="95"/>
       <c r="B25" s="93"/>
       <c r="C25" s="93"/>
@@ -6247,7 +6270,7 @@
       <c r="J25" s="80"/>
       <c r="K25" s="80"/>
     </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A26" s="95"/>
       <c r="B26" s="93"/>
       <c r="C26" s="93"/>
@@ -6260,7 +6283,7 @@
       <c r="J26" s="80"/>
       <c r="K26" s="80"/>
     </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A27" s="95"/>
       <c r="B27" s="93"/>
       <c r="C27" s="93"/>
@@ -6273,7 +6296,7 @@
       <c r="J27" s="80"/>
       <c r="K27" s="80"/>
     </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A28" s="98"/>
       <c r="B28" s="98"/>
       <c r="C28" s="98"/>
@@ -6286,7 +6309,7 @@
       <c r="J28" s="80"/>
       <c r="K28" s="80"/>
     </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A29" s="80"/>
       <c r="B29" s="80"/>
       <c r="C29" s="80"/>
@@ -6299,7 +6322,7 @@
       <c r="J29" s="80"/>
       <c r="K29" s="80"/>
     </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A30" s="80"/>
       <c r="B30" s="80"/>
       <c r="C30" s="80"/>
@@ -6312,7 +6335,7 @@
       <c r="J30" s="80"/>
       <c r="K30" s="80"/>
     </row>
-    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A31" s="80"/>
       <c r="B31" s="80"/>
       <c r="C31" s="80"/>
@@ -6325,7 +6348,7 @@
       <c r="J31" s="80"/>
       <c r="K31" s="80"/>
     </row>
-    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A32" s="80"/>
       <c r="B32" s="80"/>
       <c r="C32" s="80"/>
@@ -6338,7 +6361,7 @@
       <c r="J32" s="80"/>
       <c r="K32" s="80"/>
     </row>
-    <row r="33" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A33" s="80"/>
       <c r="B33" s="80"/>
       <c r="C33" s="80"/>
@@ -6351,9 +6374,9 @@
       <c r="J33" s="80"/>
       <c r="K33" s="80"/>
     </row>
-    <row r="34" spans="1:11" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:11" ht="18" x14ac:dyDescent="0.3">
       <c r="A34" s="87" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="B34" s="80"/>
       <c r="C34" s="80"/>

</xml_diff>

<commit_message>
version 1.0 before gdsd approval
</commit_message>
<xml_diff>
--- a/PowerPlantProduction.xlsx
+++ b/PowerPlantProduction.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="204" yWindow="180" windowWidth="17268" windowHeight="7752"/>
+    <workbookView xWindow="210" yWindow="180" windowWidth="17265" windowHeight="7755"/>
   </bookViews>
   <sheets>
     <sheet name="About" sheetId="3" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="324" uniqueCount="202">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="327" uniqueCount="205">
   <si>
     <t>Title</t>
   </si>
@@ -667,10 +667,19 @@
     <t>The year in which the first power plant at the site began operation. Included as search parameter. Integer to help enforce 'YYYY' value.</t>
   </si>
   <si>
-    <t>update implementation data type to 'double' for Capacity_MW, GrossProduction_MWhr, NetProduction_MWhr, AveragePrice_c_kW-h; was string for a decimal data type.  This won't appear until next version release.</t>
-  </si>
-  <si>
     <t xml:space="preserve"> this is the version that is on schemas.usgin.org as version 0.8</t>
+  </si>
+  <si>
+    <t>1.0</t>
+  </si>
+  <si>
+    <t xml:space="preserve">update implementation data type to 'double' for Capacity_MW, GrossProduction_MWhr, NetProduction_MWhr, AveragePrice_c_kW-h; was string for a decimal data type. </t>
+  </si>
+  <si>
+    <t>Versioning before approval by gdsdpwg. No services yet use this content model.</t>
+  </si>
+  <si>
+    <t>Christy Caudill</t>
   </si>
 </sst>
 </file>
@@ -2293,7 +2302,7 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="158">
+  <cellXfs count="159">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
@@ -2766,6 +2775,9 @@
     </xf>
     <xf numFmtId="0" fontId="30" fillId="58" borderId="39" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="355">
@@ -3570,18 +3582,18 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="C2:F34"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B8" workbookViewId="0">
-      <selection activeCell="E17" sqref="E17"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="2" width="9.109375" style="72"/>
-    <col min="3" max="3" width="12.44140625" style="71" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="66.109375" style="72" customWidth="1"/>
-    <col min="5" max="5" width="22.5546875" style="72" customWidth="1"/>
-    <col min="6" max="6" width="11.88671875" style="72" customWidth="1"/>
-    <col min="7" max="16384" width="9.109375" style="72"/>
+    <col min="1" max="2" width="9.140625" style="72"/>
+    <col min="3" max="3" width="12.42578125" style="71" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="66.140625" style="72" customWidth="1"/>
+    <col min="5" max="5" width="22.5703125" style="72" customWidth="1"/>
+    <col min="6" max="6" width="11.85546875" style="72" customWidth="1"/>
+    <col min="7" max="16384" width="9.140625" style="72"/>
   </cols>
   <sheetData>
     <row r="2" spans="3:6" ht="105.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -3593,12 +3605,12 @@
         <v>102</v>
       </c>
     </row>
-    <row r="4" spans="3:6" ht="15" x14ac:dyDescent="0.25">
+    <row r="4" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C4" s="70" t="s">
         <v>1</v>
       </c>
       <c r="D4" s="68" t="s">
-        <v>103</v>
+        <v>201</v>
       </c>
     </row>
     <row r="5" spans="3:6" ht="75" x14ac:dyDescent="0.25">
@@ -3617,10 +3629,10 @@
         <v>67</v>
       </c>
     </row>
-    <row r="7" spans="3:6" ht="15" x14ac:dyDescent="0.25">
+    <row r="7" spans="3:6" x14ac:dyDescent="0.25">
       <c r="D7" s="66"/>
     </row>
-    <row r="9" spans="3:6" ht="15" x14ac:dyDescent="0.25">
+    <row r="9" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C9" s="65" t="s">
         <v>4</v>
       </c>
@@ -3648,7 +3660,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="11" spans="3:6" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="11" spans="3:6" ht="75" x14ac:dyDescent="0.25">
       <c r="C11" s="63" t="s">
         <v>66</v>
       </c>
@@ -3662,7 +3674,7 @@
         <v>41087</v>
       </c>
     </row>
-    <row r="12" spans="3:6" x14ac:dyDescent="0.3">
+    <row r="12" spans="3:6" ht="14.45" x14ac:dyDescent="0.3">
       <c r="C12" s="63" t="s">
         <v>103</v>
       </c>
@@ -3676,10 +3688,10 @@
         <v>41180</v>
       </c>
     </row>
-    <row r="13" spans="3:6" x14ac:dyDescent="0.3">
+    <row r="13" spans="3:6" ht="14.45" x14ac:dyDescent="0.3">
       <c r="C13" s="63"/>
       <c r="D13" s="74" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="E13" s="75"/>
       <c r="F13" s="60"/>
@@ -3696,10 +3708,12 @@
         <v>41299</v>
       </c>
     </row>
-    <row r="15" spans="3:6" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="C15" s="63"/>
+    <row r="15" spans="3:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="C15" s="63" t="s">
+        <v>201</v>
+      </c>
       <c r="D15" s="74" t="s">
-        <v>200</v>
+        <v>202</v>
       </c>
       <c r="E15" s="73" t="s">
         <v>95</v>
@@ -3708,72 +3722,78 @@
         <v>41403</v>
       </c>
     </row>
-    <row r="16" spans="3:6" x14ac:dyDescent="0.3">
+    <row r="16" spans="3:6" ht="30" x14ac:dyDescent="0.25">
       <c r="C16" s="63"/>
-      <c r="D16" s="75"/>
-      <c r="E16" s="75"/>
-      <c r="F16" s="60"/>
-    </row>
-    <row r="17" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="D16" s="158" t="s">
+        <v>203</v>
+      </c>
+      <c r="E16" s="75" t="s">
+        <v>204</v>
+      </c>
+      <c r="F16" s="60">
+        <v>41409</v>
+      </c>
+    </row>
+    <row r="17" spans="3:6" ht="14.45" x14ac:dyDescent="0.3">
       <c r="C17" s="63"/>
       <c r="D17" s="75"/>
       <c r="E17" s="75"/>
       <c r="F17" s="60"/>
     </row>
-    <row r="18" spans="3:6" x14ac:dyDescent="0.3">
+    <row r="18" spans="3:6" ht="14.45" x14ac:dyDescent="0.3">
       <c r="C18" s="63"/>
       <c r="D18" s="75"/>
       <c r="E18" s="75"/>
       <c r="F18" s="60"/>
     </row>
-    <row r="19" spans="3:6" x14ac:dyDescent="0.3">
+    <row r="19" spans="3:6" ht="14.45" x14ac:dyDescent="0.3">
       <c r="C19" s="63"/>
       <c r="D19" s="75"/>
       <c r="E19" s="75"/>
       <c r="F19" s="60"/>
     </row>
-    <row r="20" spans="3:6" x14ac:dyDescent="0.3">
+    <row r="20" spans="3:6" ht="14.45" x14ac:dyDescent="0.3">
       <c r="C20" s="63"/>
       <c r="D20" s="75"/>
       <c r="E20" s="75"/>
       <c r="F20" s="60"/>
     </row>
-    <row r="21" spans="3:6" x14ac:dyDescent="0.3">
+    <row r="21" spans="3:6" ht="14.45" x14ac:dyDescent="0.3">
       <c r="C21" s="63"/>
       <c r="D21" s="75"/>
       <c r="E21" s="75"/>
       <c r="F21" s="60"/>
     </row>
-    <row r="22" spans="3:6" x14ac:dyDescent="0.3">
+    <row r="22" spans="3:6" ht="14.45" x14ac:dyDescent="0.3">
       <c r="C22" s="70"/>
       <c r="D22" s="75"/>
       <c r="E22" s="75"/>
       <c r="F22" s="60"/>
     </row>
-    <row r="23" spans="3:6" x14ac:dyDescent="0.3">
+    <row r="23" spans="3:6" ht="14.45" x14ac:dyDescent="0.3">
       <c r="C23" s="70"/>
       <c r="D23" s="75"/>
       <c r="E23" s="75"/>
       <c r="F23" s="60"/>
     </row>
-    <row r="25" spans="3:6" x14ac:dyDescent="0.3">
+    <row r="25" spans="3:6" x14ac:dyDescent="0.25">
       <c r="D25" s="118" t="s">
         <v>197</v>
       </c>
     </row>
-    <row r="26" spans="3:6" x14ac:dyDescent="0.3">
+    <row r="26" spans="3:6" x14ac:dyDescent="0.25">
       <c r="D26" s="119" t="s">
         <v>198</v>
       </c>
     </row>
-    <row r="29" spans="3:6" ht="18" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="29" spans="3:6" ht="18" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C29" s="72"/>
       <c r="D29" s="59" t="s">
         <v>155</v>
       </c>
       <c r="E29" s="58"/>
     </row>
-    <row r="30" spans="3:6" ht="15" thickTop="1" x14ac:dyDescent="0.3">
+    <row r="30" spans="3:6" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="C30" s="57"/>
       <c r="D30" s="56" t="s">
         <v>5</v>
@@ -3785,25 +3805,25 @@
         <v>7</v>
       </c>
     </row>
-    <row r="31" spans="3:6" x14ac:dyDescent="0.3">
+    <row r="31" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C31" s="72"/>
       <c r="D31" s="73"/>
       <c r="E31" s="74"/>
       <c r="F31" s="73"/>
     </row>
-    <row r="32" spans="3:6" x14ac:dyDescent="0.3">
+    <row r="32" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C32" s="72"/>
       <c r="D32" s="73"/>
       <c r="E32" s="74"/>
       <c r="F32" s="73"/>
     </row>
-    <row r="33" spans="3:6" x14ac:dyDescent="0.3">
+    <row r="33" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C33" s="72"/>
       <c r="D33" s="73"/>
       <c r="E33" s="74"/>
       <c r="F33" s="73"/>
     </row>
-    <row r="34" spans="3:6" x14ac:dyDescent="0.3">
+    <row r="34" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C34" s="72"/>
       <c r="D34" s="73"/>
       <c r="E34" s="74"/>
@@ -3828,12 +3848,12 @@
       <selection activeCell="B20" sqref="B20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="29.109375" style="1" customWidth="1"/>
-    <col min="2" max="2" width="63.109375" style="3" customWidth="1"/>
-    <col min="3" max="3" width="37.6640625" style="1" customWidth="1"/>
-    <col min="4" max="16384" width="8.88671875" style="1"/>
+    <col min="1" max="1" width="29.140625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="63.140625" style="3" customWidth="1"/>
+    <col min="3" max="3" width="37.7109375" style="1" customWidth="1"/>
+    <col min="4" max="16384" width="8.85546875" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="20.25" thickBot="1" x14ac:dyDescent="0.3">
@@ -3856,14 +3876,14 @@
       <c r="E2" s="2"/>
       <c r="F2" s="2"/>
     </row>
-    <row r="4" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="109" t="s">
         <v>174</v>
       </c>
       <c r="B4" s="114"/>
       <c r="C4" s="103"/>
     </row>
-    <row r="5" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="104" t="s">
         <v>175</v>
       </c>
@@ -3886,7 +3906,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="8" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="111" t="s">
         <v>179</v>
       </c>
@@ -3916,77 +3936,77 @@
       <c r="B11" s="108"/>
       <c r="C11" s="116"/>
     </row>
-    <row r="12" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" s="104" t="s">
         <v>184</v>
       </c>
       <c r="B12" s="112"/>
       <c r="C12" s="103"/>
     </row>
-    <row r="13" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" s="104" t="s">
         <v>185</v>
       </c>
       <c r="B13" s="104"/>
       <c r="C13" s="103"/>
     </row>
-    <row r="14" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" s="104" t="s">
         <v>186</v>
       </c>
       <c r="B14" s="104"/>
       <c r="C14" s="103"/>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:6" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A15" s="104" t="s">
         <v>187</v>
       </c>
       <c r="B15" s="104"/>
       <c r="C15" s="103"/>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:6" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A16" s="104" t="s">
         <v>188</v>
       </c>
       <c r="B16" s="104"/>
       <c r="C16" s="103"/>
     </row>
-    <row r="17" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:3" ht="28.9" x14ac:dyDescent="0.3">
       <c r="A17" s="104" t="s">
         <v>189</v>
       </c>
       <c r="B17" s="104"/>
       <c r="C17" s="103"/>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" s="104" t="s">
         <v>190</v>
       </c>
       <c r="B18" s="104"/>
       <c r="C18" s="80"/>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" s="104" t="s">
         <v>191</v>
       </c>
       <c r="B19" s="104"/>
       <c r="C19" s="80"/>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" s="104" t="s">
         <v>192</v>
       </c>
       <c r="B20" s="104"/>
       <c r="C20" s="80"/>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" s="104" t="s">
         <v>9</v>
       </c>
       <c r="B21" s="104"/>
       <c r="C21" s="80"/>
     </row>
-    <row r="22" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A22" s="104" t="s">
         <v>193</v>
       </c>
@@ -4010,41 +4030,41 @@
   <dimension ref="A1:AC53"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A26" sqref="A26"/>
+      <selection activeCell="AC1" sqref="AC1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="80.33203125" style="125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="26.5546875" style="125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="62.44140625" style="125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.33203125" style="125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="80.28515625" style="125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="26.5703125" style="125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="62.42578125" style="125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.28515625" style="125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="12" style="125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="5.88671875" style="125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="12.44140625" style="125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="17.44140625" style="125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="9.6640625" style="125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="10.6640625" style="125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="14.5546875" style="125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="35.5546875" style="125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.140625" style="125" customWidth="1"/>
+    <col min="7" max="7" width="12.42578125" style="125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="17.42578125" style="125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="9.7109375" style="125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="10.7109375" style="125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="14.5703125" style="125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="35.5703125" style="125" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="10" style="128" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="5.44140625" style="125" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="9.5546875" style="125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="5.42578125" style="125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="9.5703125" style="125" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="11" style="126" bestFit="1" customWidth="1"/>
     <col min="17" max="17" width="10" style="125" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="26.5546875" style="125" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="26.5703125" style="125" bestFit="1" customWidth="1"/>
     <col min="19" max="19" width="19" style="125" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="16.44140625" style="128" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="16.109375" style="128" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="10.44140625" style="125" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="12.6640625" style="125" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="21.33203125" style="125" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="19.109375" style="129" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="19.5546875" style="129" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="217.33203125" style="125" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="11.6640625" style="125" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="16.44140625" style="125" bestFit="1" customWidth="1"/>
-    <col min="30" max="16384" width="9.109375" style="125"/>
+    <col min="20" max="20" width="16.42578125" style="128" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="16.140625" style="128" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="10.42578125" style="125" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="12.7109375" style="125" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="21.28515625" style="125" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="19.140625" style="129" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="19.5703125" style="129" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="217.28515625" style="125" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="11.7109375" style="125" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="16.42578125" style="125" bestFit="1" customWidth="1"/>
+    <col min="30" max="16384" width="9.140625" style="125"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:29" s="120" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -4479,7 +4499,7 @@
       <c r="Y8" s="125"/>
       <c r="Z8" s="125"/>
     </row>
-    <row r="9" spans="1:29" ht="15" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:29" x14ac:dyDescent="0.25">
       <c r="C9" s="126"/>
       <c r="D9" s="143"/>
       <c r="I9" s="127"/>
@@ -4490,7 +4510,7 @@
       <c r="Y9" s="125"/>
       <c r="Z9" s="125"/>
     </row>
-    <row r="10" spans="1:29" ht="15" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:29" x14ac:dyDescent="0.25">
       <c r="C10" s="126"/>
       <c r="D10" s="143"/>
       <c r="I10" s="127"/>
@@ -4501,7 +4521,7 @@
       <c r="Y10" s="125"/>
       <c r="Z10" s="125"/>
     </row>
-    <row r="11" spans="1:29" ht="15" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:29" x14ac:dyDescent="0.25">
       <c r="C11" s="126"/>
       <c r="D11" s="143"/>
       <c r="I11" s="127"/>
@@ -4512,7 +4532,7 @@
       <c r="Y11" s="125"/>
       <c r="Z11" s="125"/>
     </row>
-    <row r="12" spans="1:29" ht="15" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:29" x14ac:dyDescent="0.25">
       <c r="C12" s="126"/>
       <c r="D12" s="143"/>
       <c r="I12" s="127"/>
@@ -4523,7 +4543,7 @@
       <c r="Y12" s="125"/>
       <c r="Z12" s="125"/>
     </row>
-    <row r="13" spans="1:29" ht="15" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:29" x14ac:dyDescent="0.25">
       <c r="C13" s="126"/>
       <c r="D13" s="143"/>
       <c r="I13" s="127"/>
@@ -4534,7 +4554,7 @@
       <c r="Y13" s="125"/>
       <c r="Z13" s="125"/>
     </row>
-    <row r="14" spans="1:29" ht="15" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:29" x14ac:dyDescent="0.25">
       <c r="C14" s="144"/>
       <c r="D14" s="144"/>
       <c r="I14" s="127"/>
@@ -4545,7 +4565,7 @@
       <c r="Y14" s="125"/>
       <c r="Z14" s="125"/>
     </row>
-    <row r="15" spans="1:29" ht="15" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:29" x14ac:dyDescent="0.25">
       <c r="C15" s="144"/>
       <c r="D15" s="144"/>
       <c r="I15" s="127"/>
@@ -4556,7 +4576,7 @@
       <c r="Y15" s="125"/>
       <c r="Z15" s="125"/>
     </row>
-    <row r="16" spans="1:29" ht="15" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:29" x14ac:dyDescent="0.25">
       <c r="C16" s="126"/>
       <c r="D16" s="143"/>
       <c r="I16" s="127"/>
@@ -4567,7 +4587,7 @@
       <c r="Y16" s="125"/>
       <c r="Z16" s="125"/>
     </row>
-    <row r="17" spans="3:21" s="125" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+    <row r="17" spans="3:21" s="125" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C17" s="126"/>
       <c r="D17" s="143"/>
       <c r="I17" s="127"/>
@@ -4576,7 +4596,7 @@
       <c r="T17" s="128"/>
       <c r="U17" s="128"/>
     </row>
-    <row r="18" spans="3:21" s="125" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+    <row r="18" spans="3:21" s="125" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C18" s="126"/>
       <c r="D18" s="143"/>
       <c r="I18" s="127"/>
@@ -4585,7 +4605,7 @@
       <c r="T18" s="128"/>
       <c r="U18" s="128"/>
     </row>
-    <row r="19" spans="3:21" s="125" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+    <row r="19" spans="3:21" s="125" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C19" s="126"/>
       <c r="D19" s="143"/>
       <c r="I19" s="127"/>
@@ -4594,7 +4614,7 @@
       <c r="T19" s="128"/>
       <c r="U19" s="128"/>
     </row>
-    <row r="20" spans="3:21" s="125" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="3:21" s="125" customFormat="1" ht="14.45" x14ac:dyDescent="0.3">
       <c r="C20" s="126"/>
       <c r="D20" s="143"/>
       <c r="I20" s="127"/>
@@ -4603,7 +4623,7 @@
       <c r="T20" s="128"/>
       <c r="U20" s="128"/>
     </row>
-    <row r="21" spans="3:21" s="125" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="3:21" s="125" customFormat="1" ht="14.45" x14ac:dyDescent="0.3">
       <c r="C21" s="144"/>
       <c r="D21" s="144"/>
       <c r="I21" s="127"/>
@@ -4612,7 +4632,7 @@
       <c r="T21" s="128"/>
       <c r="U21" s="128"/>
     </row>
-    <row r="22" spans="3:21" s="125" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="3:21" s="125" customFormat="1" ht="14.45" x14ac:dyDescent="0.3">
       <c r="C22" s="126"/>
       <c r="D22" s="143"/>
       <c r="I22" s="127"/>
@@ -4621,14 +4641,14 @@
       <c r="T22" s="128"/>
       <c r="U22" s="128"/>
     </row>
-    <row r="23" spans="3:21" s="125" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="3:21" s="125" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C23" s="126"/>
       <c r="D23" s="143"/>
       <c r="N23" s="127"/>
       <c r="T23" s="128"/>
       <c r="U23" s="128"/>
     </row>
-    <row r="24" spans="3:21" s="125" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="24" spans="3:21" s="125" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C24" s="126"/>
       <c r="D24" s="143"/>
       <c r="I24" s="127"/>
@@ -4637,7 +4657,7 @@
       <c r="T24" s="128"/>
       <c r="U24" s="128"/>
     </row>
-    <row r="25" spans="3:21" s="125" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="25" spans="3:21" s="125" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C25" s="126"/>
       <c r="D25" s="143"/>
       <c r="I25" s="127"/>
@@ -4646,7 +4666,7 @@
       <c r="T25" s="128"/>
       <c r="U25" s="128"/>
     </row>
-    <row r="26" spans="3:21" s="125" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="26" spans="3:21" s="125" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C26" s="126"/>
       <c r="D26" s="143"/>
       <c r="I26" s="127"/>
@@ -4655,7 +4675,7 @@
       <c r="T26" s="128"/>
       <c r="U26" s="128"/>
     </row>
-    <row r="27" spans="3:21" s="125" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="27" spans="3:21" s="125" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C27" s="126"/>
       <c r="D27" s="143"/>
       <c r="I27" s="127"/>
@@ -4664,7 +4684,7 @@
       <c r="T27" s="128"/>
       <c r="U27" s="128"/>
     </row>
-    <row r="28" spans="3:21" s="125" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="28" spans="3:21" s="125" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C28" s="126"/>
       <c r="D28" s="143"/>
       <c r="I28" s="127"/>
@@ -4673,7 +4693,7 @@
       <c r="T28" s="128"/>
       <c r="U28" s="128"/>
     </row>
-    <row r="29" spans="3:21" s="125" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="29" spans="3:21" s="125" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C29" s="126"/>
       <c r="D29" s="143"/>
       <c r="I29" s="127"/>
@@ -4682,7 +4702,7 @@
       <c r="T29" s="128"/>
       <c r="U29" s="128"/>
     </row>
-    <row r="30" spans="3:21" s="125" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="30" spans="3:21" s="125" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C30" s="144"/>
       <c r="D30" s="144"/>
       <c r="I30" s="127"/>
@@ -4691,7 +4711,7 @@
       <c r="T30" s="128"/>
       <c r="U30" s="128"/>
     </row>
-    <row r="31" spans="3:21" s="125" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="31" spans="3:21" s="125" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C31" s="144"/>
       <c r="D31" s="144"/>
       <c r="I31" s="127"/>
@@ -4700,7 +4720,7 @@
       <c r="T31" s="128"/>
       <c r="U31" s="128"/>
     </row>
-    <row r="32" spans="3:21" s="125" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="32" spans="3:21" s="125" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C32" s="126"/>
       <c r="D32" s="143"/>
       <c r="I32" s="127"/>
@@ -4709,7 +4729,7 @@
       <c r="T32" s="128"/>
       <c r="U32" s="128"/>
     </row>
-    <row r="33" spans="3:21" s="125" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="33" spans="3:21" s="125" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C33" s="126"/>
       <c r="D33" s="143"/>
       <c r="I33" s="127"/>
@@ -4718,7 +4738,7 @@
       <c r="T33" s="128"/>
       <c r="U33" s="128"/>
     </row>
-    <row r="34" spans="3:21" s="125" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="34" spans="3:21" s="125" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C34" s="126"/>
       <c r="D34" s="143"/>
       <c r="I34" s="127"/>
@@ -4727,7 +4747,7 @@
       <c r="T34" s="128"/>
       <c r="U34" s="128"/>
     </row>
-    <row r="35" spans="3:21" s="125" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="35" spans="3:21" s="125" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C35" s="126"/>
       <c r="D35" s="143"/>
       <c r="I35" s="127"/>
@@ -4736,7 +4756,7 @@
       <c r="T35" s="128"/>
       <c r="U35" s="128"/>
     </row>
-    <row r="36" spans="3:21" s="125" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="36" spans="3:21" s="125" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C36" s="126"/>
       <c r="D36" s="143"/>
       <c r="I36" s="127"/>
@@ -4745,7 +4765,7 @@
       <c r="T36" s="128"/>
       <c r="U36" s="128"/>
     </row>
-    <row r="37" spans="3:21" s="125" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="37" spans="3:21" s="125" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C37" s="144"/>
       <c r="D37" s="144"/>
       <c r="I37" s="127"/>
@@ -4754,7 +4774,7 @@
       <c r="T37" s="128"/>
       <c r="U37" s="128"/>
     </row>
-    <row r="38" spans="3:21" s="125" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="38" spans="3:21" s="125" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C38" s="126"/>
       <c r="D38" s="143"/>
       <c r="I38" s="127"/>
@@ -4763,66 +4783,66 @@
       <c r="T38" s="128"/>
       <c r="U38" s="128"/>
     </row>
-    <row r="39" spans="3:21" s="125" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="39" spans="3:21" s="125" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C39" s="126"/>
       <c r="D39" s="143"/>
       <c r="N39" s="127"/>
       <c r="T39" s="128"/>
       <c r="U39" s="128"/>
     </row>
-    <row r="40" spans="3:21" s="125" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="40" spans="3:21" s="125" customFormat="1" x14ac:dyDescent="0.25">
       <c r="T40" s="128"/>
       <c r="U40" s="128"/>
     </row>
-    <row r="41" spans="3:21" s="125" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="41" spans="3:21" s="125" customFormat="1" x14ac:dyDescent="0.25">
       <c r="T41" s="128"/>
       <c r="U41" s="128"/>
     </row>
-    <row r="42" spans="3:21" s="125" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="42" spans="3:21" s="125" customFormat="1" x14ac:dyDescent="0.25">
       <c r="T42" s="128"/>
       <c r="U42" s="128"/>
     </row>
-    <row r="43" spans="3:21" s="125" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="43" spans="3:21" s="125" customFormat="1" x14ac:dyDescent="0.25">
       <c r="T43" s="128"/>
       <c r="U43" s="128"/>
     </row>
-    <row r="44" spans="3:21" s="125" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="44" spans="3:21" s="125" customFormat="1" x14ac:dyDescent="0.25">
       <c r="T44" s="128"/>
       <c r="U44" s="128"/>
     </row>
-    <row r="45" spans="3:21" s="125" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="45" spans="3:21" s="125" customFormat="1" x14ac:dyDescent="0.25">
       <c r="T45" s="128"/>
       <c r="U45" s="128"/>
     </row>
-    <row r="46" spans="3:21" s="125" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="46" spans="3:21" s="125" customFormat="1" x14ac:dyDescent="0.25">
       <c r="T46" s="128"/>
       <c r="U46" s="128"/>
     </row>
-    <row r="47" spans="3:21" s="125" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="47" spans="3:21" s="125" customFormat="1" x14ac:dyDescent="0.25">
       <c r="T47" s="128"/>
       <c r="U47" s="128"/>
     </row>
-    <row r="48" spans="3:21" s="125" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="48" spans="3:21" s="125" customFormat="1" x14ac:dyDescent="0.25">
       <c r="T48" s="128"/>
       <c r="U48" s="128"/>
     </row>
-    <row r="49" spans="20:21" s="125" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="49" spans="20:21" s="125" customFormat="1" x14ac:dyDescent="0.25">
       <c r="T49" s="128"/>
       <c r="U49" s="128"/>
     </row>
-    <row r="50" spans="20:21" s="125" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="50" spans="20:21" s="125" customFormat="1" x14ac:dyDescent="0.25">
       <c r="T50" s="128"/>
       <c r="U50" s="128"/>
     </row>
-    <row r="51" spans="20:21" s="125" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="51" spans="20:21" s="125" customFormat="1" x14ac:dyDescent="0.25">
       <c r="T51" s="128"/>
       <c r="U51" s="128"/>
     </row>
-    <row r="52" spans="20:21" s="125" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="52" spans="20:21" s="125" customFormat="1" x14ac:dyDescent="0.25">
       <c r="T52" s="128"/>
       <c r="U52" s="128"/>
     </row>
-    <row r="53" spans="20:21" s="125" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="53" spans="20:21" s="125" customFormat="1" x14ac:dyDescent="0.25">
       <c r="T53" s="128"/>
       <c r="U53" s="128"/>
     </row>
@@ -4850,20 +4870,20 @@
   </sheetPr>
   <dimension ref="A1:BJ34"/>
   <sheetViews>
-    <sheetView topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="A27" sqref="A27:A30"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="13.8" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="14.25" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="25.6640625" style="11" customWidth="1"/>
-    <col min="2" max="2" width="18.6640625" style="14" customWidth="1"/>
+    <col min="1" max="1" width="25.7109375" style="11" customWidth="1"/>
+    <col min="2" max="2" width="18.7109375" style="14" customWidth="1"/>
     <col min="3" max="3" width="21" style="14" customWidth="1"/>
-    <col min="4" max="4" width="15.88671875" style="14" customWidth="1"/>
-    <col min="5" max="5" width="46.88671875" style="14" customWidth="1"/>
-    <col min="6" max="6" width="39.109375" style="14" customWidth="1"/>
-    <col min="7" max="7" width="40.88671875" style="14" customWidth="1"/>
-    <col min="8" max="16384" width="9.109375" style="15"/>
+    <col min="4" max="4" width="15.85546875" style="14" customWidth="1"/>
+    <col min="5" max="5" width="46.85546875" style="14" customWidth="1"/>
+    <col min="6" max="6" width="39.140625" style="14" customWidth="1"/>
+    <col min="7" max="7" width="40.85546875" style="14" customWidth="1"/>
+    <col min="8" max="16384" width="9.140625" style="15"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:62" s="11" customFormat="1" ht="19.5" x14ac:dyDescent="0.25">
@@ -5314,7 +5334,7 @@
       <c r="F10" s="28"/>
       <c r="G10" s="23"/>
     </row>
-    <row r="11" spans="1:62" s="6" customFormat="1" ht="35.4" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:62" s="6" customFormat="1" ht="35.450000000000003" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="8" t="s">
         <v>47</v>
       </c>
@@ -5542,7 +5562,7 @@
       <c r="F22" s="24"/>
       <c r="G22" s="24"/>
     </row>
-    <row r="23" spans="1:11" s="6" customFormat="1" ht="31.2" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:11" s="6" customFormat="1" ht="31.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="29" t="s">
         <v>72</v>
       </c>
@@ -5618,7 +5638,7 @@
       <c r="F26" s="23"/>
       <c r="G26" s="23"/>
     </row>
-    <row r="27" spans="1:11" s="6" customFormat="1" ht="26.4" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:11" s="6" customFormat="1" ht="26.45" x14ac:dyDescent="0.3">
       <c r="A27" s="31" t="s">
         <v>16</v>
       </c>
@@ -5637,7 +5657,7 @@
       <c r="F27" s="23"/>
       <c r="G27" s="23"/>
     </row>
-    <row r="28" spans="1:11" s="6" customFormat="1" ht="26.4" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:11" s="6" customFormat="1" ht="26.45" x14ac:dyDescent="0.3">
       <c r="A28" s="31" t="s">
         <v>82</v>
       </c>
@@ -5656,7 +5676,7 @@
       <c r="F28" s="23"/>
       <c r="G28" s="23"/>
     </row>
-    <row r="29" spans="1:11" s="6" customFormat="1" ht="26.4" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:11" s="6" customFormat="1" ht="26.45" x14ac:dyDescent="0.3">
       <c r="A29" s="31" t="s">
         <v>83</v>
       </c>
@@ -5736,7 +5756,7 @@
       <c r="J32" s="6"/>
       <c r="K32" s="6"/>
     </row>
-    <row r="33" spans="1:10" ht="26.4" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:10" ht="26.45" x14ac:dyDescent="0.3">
       <c r="A33" s="18" t="s">
         <v>38</v>
       </c>
@@ -5758,7 +5778,7 @@
       <c r="I33" s="6"/>
       <c r="J33" s="6"/>
     </row>
-    <row r="34" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:10" ht="13.9" x14ac:dyDescent="0.3">
       <c r="A34" s="10"/>
       <c r="B34" s="17"/>
     </row>
@@ -5781,20 +5801,20 @@
       <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.109375" style="7"/>
+    <col min="1" max="1" width="9.140625" style="7"/>
     <col min="2" max="2" width="22" style="4" customWidth="1"/>
-    <col min="3" max="3" width="61.109375" style="4" customWidth="1"/>
-    <col min="4" max="4" width="55.44140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="43.109375" customWidth="1"/>
+    <col min="3" max="3" width="61.140625" style="4" customWidth="1"/>
+    <col min="4" max="4" width="55.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="43.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B1"/>
       <c r="C1"/>
     </row>
-    <row r="2" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="51" t="s">
         <v>64</v>
       </c>
@@ -5817,7 +5837,7 @@
       </c>
       <c r="E3" s="46"/>
     </row>
-    <row r="4" spans="1:5" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:5" ht="75" x14ac:dyDescent="0.25">
       <c r="A4" s="52"/>
       <c r="B4" s="52" t="s">
         <v>108</v>
@@ -5856,19 +5876,19 @@
       </c>
       <c r="E6" s="46"/>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:5" ht="14.45" x14ac:dyDescent="0.3">
       <c r="B7"/>
       <c r="C7"/>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:5" ht="14.45" x14ac:dyDescent="0.3">
       <c r="B8"/>
       <c r="C8"/>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:5" ht="14.45" x14ac:dyDescent="0.3">
       <c r="B9"/>
       <c r="C9"/>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:5" ht="14.45" x14ac:dyDescent="0.3">
       <c r="B10"/>
       <c r="C10"/>
     </row>
@@ -5892,13 +5912,13 @@
       <selection activeCell="D22" sqref="D22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="18.5546875" customWidth="1"/>
-    <col min="2" max="2" width="11.44140625" customWidth="1"/>
-    <col min="3" max="3" width="24.6640625" customWidth="1"/>
-    <col min="4" max="4" width="53.109375" customWidth="1"/>
-    <col min="5" max="9" width="16.109375" customWidth="1"/>
+    <col min="1" max="1" width="18.5703125" customWidth="1"/>
+    <col min="2" max="2" width="11.42578125" customWidth="1"/>
+    <col min="3" max="3" width="24.7109375" customWidth="1"/>
+    <col min="4" max="4" width="53.140625" customWidth="1"/>
+    <col min="5" max="9" width="16.140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="18.75" x14ac:dyDescent="0.25">
@@ -6072,7 +6092,7 @@
       <c r="J11" s="80"/>
       <c r="K11" s="80"/>
     </row>
-    <row r="12" spans="1:11" ht="15" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12" s="95"/>
       <c r="B12" s="95"/>
       <c r="C12" s="86"/>
@@ -6125,7 +6145,7 @@
       <c r="J14" s="80"/>
       <c r="K14" s="80"/>
     </row>
-    <row r="15" spans="1:11" ht="15" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A15" s="95"/>
       <c r="B15" s="93"/>
       <c r="C15" s="93"/>
@@ -6153,7 +6173,7 @@
       <c r="J16" s="80"/>
       <c r="K16" s="80"/>
     </row>
-    <row r="17" spans="1:11" ht="15" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A17" s="95"/>
       <c r="B17" s="93"/>
       <c r="C17" s="93"/>
@@ -6166,7 +6186,7 @@
       <c r="J17" s="80"/>
       <c r="K17" s="80"/>
     </row>
-    <row r="18" spans="1:11" ht="15" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A18" s="95"/>
       <c r="B18" s="93"/>
       <c r="C18" s="93"/>
@@ -6179,7 +6199,7 @@
       <c r="J18" s="80"/>
       <c r="K18" s="102"/>
     </row>
-    <row r="19" spans="1:11" ht="15" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A19" s="95"/>
       <c r="B19" s="93"/>
       <c r="C19" s="93"/>
@@ -6192,7 +6212,7 @@
       <c r="J19" s="80"/>
       <c r="K19" s="80"/>
     </row>
-    <row r="20" spans="1:11" ht="15" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A20" s="83"/>
       <c r="B20" s="93"/>
       <c r="C20" s="93"/>
@@ -6205,7 +6225,7 @@
       <c r="J20" s="80"/>
       <c r="K20" s="80"/>
     </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:11" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A21" s="95"/>
       <c r="B21" s="93"/>
       <c r="C21" s="93"/>
@@ -6218,7 +6238,7 @@
       <c r="J21" s="80"/>
       <c r="K21" s="80"/>
     </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:11" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A22" s="95"/>
       <c r="B22" s="93"/>
       <c r="C22" s="93"/>
@@ -6231,7 +6251,7 @@
       <c r="J22" s="80"/>
       <c r="K22" s="80"/>
     </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:11" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A23" s="95"/>
       <c r="B23" s="93"/>
       <c r="C23" s="93"/>
@@ -6244,7 +6264,7 @@
       <c r="J23" s="80"/>
       <c r="K23" s="80"/>
     </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A24" s="95"/>
       <c r="B24" s="93"/>
       <c r="C24" s="93"/>
@@ -6257,7 +6277,7 @@
       <c r="J24" s="80"/>
       <c r="K24" s="80"/>
     </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A25" s="95"/>
       <c r="B25" s="93"/>
       <c r="C25" s="93"/>
@@ -6270,7 +6290,7 @@
       <c r="J25" s="80"/>
       <c r="K25" s="80"/>
     </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A26" s="95"/>
       <c r="B26" s="93"/>
       <c r="C26" s="93"/>
@@ -6283,7 +6303,7 @@
       <c r="J26" s="80"/>
       <c r="K26" s="80"/>
     </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A27" s="95"/>
       <c r="B27" s="93"/>
       <c r="C27" s="93"/>
@@ -6296,7 +6316,7 @@
       <c r="J27" s="80"/>
       <c r="K27" s="80"/>
     </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A28" s="98"/>
       <c r="B28" s="98"/>
       <c r="C28" s="98"/>
@@ -6309,7 +6329,7 @@
       <c r="J28" s="80"/>
       <c r="K28" s="80"/>
     </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A29" s="80"/>
       <c r="B29" s="80"/>
       <c r="C29" s="80"/>
@@ -6322,7 +6342,7 @@
       <c r="J29" s="80"/>
       <c r="K29" s="80"/>
     </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A30" s="80"/>
       <c r="B30" s="80"/>
       <c r="C30" s="80"/>
@@ -6335,7 +6355,7 @@
       <c r="J30" s="80"/>
       <c r="K30" s="80"/>
     </row>
-    <row r="31" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A31" s="80"/>
       <c r="B31" s="80"/>
       <c r="C31" s="80"/>
@@ -6348,7 +6368,7 @@
       <c r="J31" s="80"/>
       <c r="K31" s="80"/>
     </row>
-    <row r="32" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A32" s="80"/>
       <c r="B32" s="80"/>
       <c r="C32" s="80"/>
@@ -6361,7 +6381,7 @@
       <c r="J32" s="80"/>
       <c r="K32" s="80"/>
     </row>
-    <row r="33" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A33" s="80"/>
       <c r="B33" s="80"/>
       <c r="C33" s="80"/>
@@ -6374,7 +6394,7 @@
       <c r="J33" s="80"/>
       <c r="K33" s="80"/>
     </row>
-    <row r="34" spans="1:11" ht="18" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:11" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A34" s="87" t="s">
         <v>173</v>
       </c>

</xml_diff>